<commit_message>
car accident assignment (q1-3 finished)
</commit_message>
<xml_diff>
--- a/AssignmentVictoria/Data_Car_accidents.xlsx
+++ b/AssignmentVictoria/Data_Car_accidents.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vbv\Desktop\My_documents\Teaching\Teaching\Data Science\Assignment_1_Blackboard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\Source\Repos\DataScienceAssignments2017\AssignmentVictoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="636" yWindow="0" windowWidth="19836" windowHeight="12276" tabRatio="717"/>
+    <workbookView xWindow="638" yWindow="0" windowWidth="19838" windowHeight="12278" tabRatio="717" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_196_subjects" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="14">
   <si>
     <t>Gender</t>
   </si>
@@ -65,11 +65,14 @@
   <si>
     <t>Accident</t>
   </si>
+  <si>
+    <t>BAC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -145,32 +148,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besøgt link" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,22 +510,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="3" width="11.796875" customWidth="1"/>
-    <col min="4" max="4" width="7.19921875" customWidth="1"/>
+    <col min="1" max="3" width="11.8125" customWidth="1"/>
+    <col min="4" max="4" width="7.1875" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="16.296875" customWidth="1"/>
+    <col min="6" max="6" width="16.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -539,10 +542,10 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -562,7 +565,7 @@
         <v>0.47199999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -582,7 +585,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -602,7 +605,7 @@
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -622,7 +625,7 @@
         <v>0.65200000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -642,7 +645,7 @@
         <v>0.53300000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -662,7 +665,7 @@
         <v>0.751</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -682,7 +685,7 @@
         <v>1.4830000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -702,7 +705,7 @@
         <v>1.5209999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -722,7 +725,7 @@
         <v>0.32200000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -742,7 +745,7 @@
         <v>0.76800000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -762,7 +765,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -782,7 +785,7 @@
         <v>0.13700000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -802,7 +805,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -822,7 +825,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -842,7 +845,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>16</v>
       </c>
@@ -862,7 +865,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>17</v>
       </c>
@@ -882,7 +885,7 @@
         <v>1.679</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>18</v>
       </c>
@@ -902,7 +905,7 @@
         <v>1.7330000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>19</v>
       </c>
@@ -922,7 +925,7 @@
         <v>1.278</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>20</v>
       </c>
@@ -942,7 +945,7 @@
         <v>1.31</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>21</v>
       </c>
@@ -962,7 +965,7 @@
         <v>0.106</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>22</v>
       </c>
@@ -982,7 +985,7 @@
         <v>0.26100000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>1.6819999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>1.4339999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1042,7 +1045,7 @@
         <v>1.63</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>0.161</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>1.008</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>0.19700000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1122,7 +1125,7 @@
         <v>1.228</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>1.7609999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>0.73199999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>1.768</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1202,7 +1205,7 @@
         <v>1.587</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>0.60799999999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1242,7 +1245,7 @@
         <v>0.39900000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1262,7 +1265,7 @@
         <v>0.40100000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1282,7 +1285,7 @@
         <v>1.387</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>0.40899999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1322,7 +1325,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>1.8160000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1362,7 +1365,7 @@
         <v>0.60099999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1402,7 +1405,7 @@
         <v>0.22900000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1422,7 +1425,7 @@
         <v>1.1439999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1442,7 +1445,7 @@
         <v>0.48199999999999998</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1462,7 +1465,7 @@
         <v>0.33400000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1482,7 +1485,7 @@
         <v>1.534</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1502,7 +1505,7 @@
         <v>1.427</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1522,7 +1525,7 @@
         <v>1.232</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1542,7 +1545,7 @@
         <v>0.77500000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1562,7 +1565,7 @@
         <v>0.52600000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>1.389</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>1.069</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1622,7 +1625,7 @@
         <v>0.22900000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>1.012</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>1.4910000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1682,7 +1685,7 @@
         <v>1.5209999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>1.0309999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1722,7 +1725,7 @@
         <v>1.2310000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>0.20200000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1762,7 +1765,7 @@
         <v>0.629</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1782,7 +1785,7 @@
         <v>0.47699999999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1802,7 +1805,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1822,7 +1825,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1842,7 +1845,7 @@
         <v>1.508</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1862,7 +1865,7 @@
         <v>1.597</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1882,7 +1885,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1902,7 +1905,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1922,7 +1925,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1942,7 +1945,7 @@
         <v>1.524</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1962,7 +1965,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1982,7 +1985,7 @@
         <v>0.433</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2002,7 +2005,7 @@
         <v>1.0720000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2022,7 +2025,7 @@
         <v>1.54</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2042,7 +2045,7 @@
         <v>0.58599999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2062,7 +2065,7 @@
         <v>1.34</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2082,7 +2085,7 @@
         <v>1.252</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2102,7 +2105,7 @@
         <v>1.6970000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>1.1850000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2142,7 +2145,7 @@
         <v>1.782</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2162,7 +2165,7 @@
         <v>1.0449999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2182,7 +2185,7 @@
         <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2202,7 +2205,7 @@
         <v>0.65100000000000002</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2222,7 +2225,7 @@
         <v>0.747</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2242,7 +2245,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>0.35699999999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2282,7 +2285,7 @@
         <v>1.5920000000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2302,7 +2305,7 @@
         <v>0.311</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2322,7 +2325,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>1.1619999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2362,7 +2365,7 @@
         <v>1.325</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2382,7 +2385,7 @@
         <v>0.63300000000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2402,7 +2405,7 @@
         <v>1.6719999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>1.6359999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2442,7 +2445,7 @@
         <v>1.0329999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2462,7 +2465,7 @@
         <v>0.50600000000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2482,7 +2485,7 @@
         <v>0.65800000000000003</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2502,7 +2505,7 @@
         <v>1.2649999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2522,7 +2525,7 @@
         <v>1.2290000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>1.3620000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2562,7 +2565,7 @@
         <v>0.38400000000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2582,7 +2585,7 @@
         <v>0.72899999999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2602,7 +2605,7 @@
         <v>1.631</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2622,7 +2625,7 @@
         <v>1.5109999999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2642,7 +2645,7 @@
         <v>0.36899999999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2662,7 +2665,7 @@
         <v>0.44500000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2682,7 +2685,7 @@
         <v>0.61099999999999999</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2702,7 +2705,7 @@
         <v>1.5509999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2722,7 +2725,7 @@
         <v>0.32200000000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2742,7 +2745,7 @@
         <v>0.53900000000000003</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2762,7 +2765,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2782,7 +2785,7 @@
         <v>0.23400000000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2802,7 +2805,7 @@
         <v>0.53400000000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>0.71199999999999997</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2842,7 +2845,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2862,7 +2865,7 @@
         <v>0.498</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2882,7 +2885,7 @@
         <v>0.38900000000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2902,7 +2905,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2922,7 +2925,7 @@
         <v>0.316</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2942,7 +2945,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2962,7 +2965,7 @@
         <v>0.28799999999999998</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2982,7 +2985,7 @@
         <v>1.623</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3002,7 +3005,7 @@
         <v>0.57299999999999995</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3022,7 +3025,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3042,7 +3045,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>0.71199999999999997</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3082,7 +3085,7 @@
         <v>0.40500000000000003</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3102,7 +3105,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3142,7 +3145,7 @@
         <v>0.26600000000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3162,7 +3165,7 @@
         <v>1.478</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3182,7 +3185,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3202,7 +3205,7 @@
         <v>0.65200000000000002</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3222,7 +3225,7 @@
         <v>0.307</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3242,7 +3245,7 @@
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3262,7 +3265,7 @@
         <v>1.706</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3282,7 +3285,7 @@
         <v>0.58899999999999997</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3302,7 +3305,7 @@
         <v>0.66600000000000004</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A140">
         <v>139</v>
       </c>
@@ -3322,7 +3325,7 @@
         <v>0.46800000000000003</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A141">
         <v>140</v>
       </c>
@@ -3342,7 +3345,7 @@
         <v>0.498</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A142">
         <v>141</v>
       </c>
@@ -3362,7 +3365,7 @@
         <v>1.599</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A143">
         <v>142</v>
       </c>
@@ -3382,7 +3385,7 @@
         <v>0.33900000000000002</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A144">
         <v>143</v>
       </c>
@@ -3402,7 +3405,7 @@
         <v>0.34200000000000003</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3422,7 +3425,7 @@
         <v>0.59899999999999998</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A146">
         <v>145</v>
       </c>
@@ -3442,7 +3445,7 @@
         <v>0.114</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A147">
         <v>146</v>
       </c>
@@ -3462,7 +3465,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A148">
         <v>147</v>
       </c>
@@ -3482,7 +3485,7 @@
         <v>1.621</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A149">
         <v>148</v>
       </c>
@@ -3502,7 +3505,7 @@
         <v>0.45500000000000002</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A150">
         <v>149</v>
       </c>
@@ -3522,7 +3525,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A151">
         <v>150</v>
       </c>
@@ -3542,7 +3545,7 @@
         <v>0.42799999999999999</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A152">
         <v>151</v>
       </c>
@@ -3562,7 +3565,7 @@
         <v>0.32300000000000001</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A153">
         <v>152</v>
       </c>
@@ -3582,7 +3585,7 @@
         <v>0.86599999999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A154">
         <v>153</v>
       </c>
@@ -3602,7 +3605,7 @@
         <v>1.359</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A155">
         <v>154</v>
       </c>
@@ -3622,7 +3625,7 @@
         <v>1.288</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A156">
         <v>155</v>
       </c>
@@ -3642,7 +3645,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A157">
         <v>156</v>
       </c>
@@ -3662,7 +3665,7 @@
         <v>0.23400000000000001</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A158">
         <v>157</v>
       </c>
@@ -3682,7 +3685,7 @@
         <v>0.25900000000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A159">
         <v>158</v>
       </c>
@@ -3702,7 +3705,7 @@
         <v>1.667</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A160">
         <v>159</v>
       </c>
@@ -3722,7 +3725,7 @@
         <v>0.68700000000000006</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A161">
         <v>160</v>
       </c>
@@ -3742,7 +3745,7 @@
         <v>0.253</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A162">
         <v>161</v>
       </c>
@@ -3762,7 +3765,7 @@
         <v>0.216</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A163">
         <v>162</v>
       </c>
@@ -3782,7 +3785,7 @@
         <v>0.68700000000000006</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A164">
         <v>163</v>
       </c>
@@ -3802,7 +3805,7 @@
         <v>1.5409999999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A165">
         <v>164</v>
       </c>
@@ -3822,7 +3825,7 @@
         <v>0.751</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A166">
         <v>165</v>
       </c>
@@ -3842,7 +3845,7 @@
         <v>0.443</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A167">
         <v>166</v>
       </c>
@@ -3862,7 +3865,7 @@
         <v>1.2709999999999999</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A168">
         <v>167</v>
       </c>
@@ -3882,7 +3885,7 @@
         <v>0.247</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A169">
         <v>168</v>
       </c>
@@ -3902,7 +3905,7 @@
         <v>0.68600000000000005</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A170">
         <v>169</v>
       </c>
@@ -3922,7 +3925,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A171">
         <v>170</v>
       </c>
@@ -3942,7 +3945,7 @@
         <v>0.26900000000000002</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A172">
         <v>171</v>
       </c>
@@ -3962,7 +3965,7 @@
         <v>0.747</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A173">
         <v>172</v>
       </c>
@@ -3982,7 +3985,7 @@
         <v>0.46300000000000002</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A174">
         <v>173</v>
       </c>
@@ -4002,7 +4005,7 @@
         <v>0.38600000000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A175">
         <v>174</v>
       </c>
@@ -4022,7 +4025,7 @@
         <v>1.3680000000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A176">
         <v>175</v>
       </c>
@@ -4042,7 +4045,7 @@
         <v>1.042</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A177">
         <v>176</v>
       </c>
@@ -4062,7 +4065,7 @@
         <v>1.0309999999999999</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A178">
         <v>177</v>
       </c>
@@ -4082,7 +4085,7 @@
         <v>0.33800000000000002</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A179">
         <v>178</v>
       </c>
@@ -4102,7 +4105,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A180">
         <v>179</v>
       </c>
@@ -4122,7 +4125,7 @@
         <v>1.5840000000000001</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A181">
         <v>180</v>
       </c>
@@ -4142,7 +4145,7 @@
         <v>1.772</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A182">
         <v>181</v>
       </c>
@@ -4162,7 +4165,7 @@
         <v>0.30199999999999999</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A183">
         <v>182</v>
       </c>
@@ -4182,7 +4185,7 @@
         <v>0.80300000000000005</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A184">
         <v>183</v>
       </c>
@@ -4202,7 +4205,7 @@
         <v>0.39700000000000002</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A185">
         <v>184</v>
       </c>
@@ -4222,7 +4225,7 @@
         <v>0.433</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A186">
         <v>185</v>
       </c>
@@ -4242,7 +4245,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A187">
         <v>186</v>
       </c>
@@ -4262,7 +4265,7 @@
         <v>0.379</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A188">
         <v>187</v>
       </c>
@@ -4282,7 +4285,7 @@
         <v>0.441</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A189">
         <v>188</v>
       </c>
@@ -4302,7 +4305,7 @@
         <v>1.3480000000000001</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A190">
         <v>189</v>
       </c>
@@ -4322,7 +4325,7 @@
         <v>0.45900000000000002</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A191">
         <v>190</v>
       </c>
@@ -4342,7 +4345,7 @@
         <v>1.732</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A192">
         <v>191</v>
       </c>
@@ -4362,7 +4365,7 @@
         <v>0.51400000000000001</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A193">
         <v>192</v>
       </c>
@@ -4382,7 +4385,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A194">
         <v>193</v>
       </c>
@@ -4402,7 +4405,7 @@
         <v>0.41799999999999998</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A195">
         <v>194</v>
       </c>
@@ -4422,7 +4425,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A196">
         <v>195</v>
       </c>
@@ -4442,7 +4445,7 @@
         <v>1.196</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A197">
         <v>196</v>
       </c>
@@ -4474,19 +4477,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="5" max="5" width="21.19921875" customWidth="1"/>
+    <col min="5" max="5" width="21.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -4506,7 +4509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>197</v>
       </c>
@@ -4526,7 +4529,7 @@
         <v>1.2070000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>198</v>
       </c>
@@ -4546,7 +4549,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>199</v>
       </c>
@@ -4566,7 +4569,7 @@
         <v>0.99399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>200</v>
       </c>
@@ -4586,7 +4589,7 @@
         <v>1.28</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>201</v>
       </c>
@@ -4606,7 +4609,7 @@
         <v>1.0289999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>202</v>
       </c>
@@ -4626,7 +4629,7 @@
         <v>1.8919999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>203</v>
       </c>
@@ -4646,7 +4649,7 @@
         <v>1.157</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>204</v>
       </c>
@@ -4666,7 +4669,7 @@
         <v>0.253</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>205</v>
       </c>
@@ -4686,7 +4689,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>206</v>
       </c>
@@ -4706,7 +4709,7 @@
         <v>1.2430000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>207</v>
       </c>
@@ -4726,7 +4729,7 @@
         <v>0.14699999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>208</v>
       </c>
@@ -4746,7 +4749,7 @@
         <v>1.9379999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>209</v>
       </c>
@@ -4766,7 +4769,7 @@
         <v>0.68899999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>210</v>
       </c>
@@ -4786,7 +4789,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>211</v>
       </c>
@@ -4806,7 +4809,7 @@
         <v>0.57399999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>212</v>
       </c>
@@ -4826,7 +4829,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>213</v>
       </c>

</xml_diff>

<commit_message>
victorias assignment (exercise 5 is wierd)
</commit_message>
<xml_diff>
--- a/AssignmentVictoria/Data_Car_accidents.xlsx
+++ b/AssignmentVictoria/Data_Car_accidents.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="638" yWindow="0" windowWidth="19838" windowHeight="12278" tabRatio="717" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="638" yWindow="0" windowWidth="19838" windowHeight="12278" tabRatio="717" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_196_subjects" sheetId="1" r:id="rId1"/>
     <sheet name="Data_17_subjects" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="13">
   <si>
     <t>Gender</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>BAC_‰</t>
-  </si>
-  <si>
     <t>Accident</t>
   </si>
   <si>
@@ -72,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -176,8 +173,36 @@
     <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{90687CA9-041E-4653-B03E-22BCA07115F1}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -513,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -533,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -542,7 +567,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">
@@ -4480,8 +4505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -4497,7 +4522,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -4506,7 +4531,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.5">

</xml_diff>